<commit_message>
more on gantt R
</commit_message>
<xml_diff>
--- a/gantt-tj3/gantt-tj3.xlsx
+++ b/gantt-tj3/gantt-tj3.xlsx
@@ -17,7 +17,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+  <si>
+    <t>Container_Task</t>
+  </si>
   <si>
     <t>task_id</t>
   </si>
@@ -34,6 +37,9 @@
     <t>BLOCKER</t>
   </si>
   <si>
+    <t>Phase1</t>
+  </si>
+  <si>
     <t>Test tj3 A</t>
   </si>
   <si>
@@ -50,6 +56,9 @@
   </si>
   <si>
     <t>previous-sibling</t>
+  </si>
+  <si>
+    <t>Phase2</t>
   </si>
   <si>
     <t>Test 2 tj3</t>
@@ -158,14 +167,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D5" activeCellId="0" pane="topLeft" sqref="D5"/>
+      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -175,70 +184,85 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="n">
         <v>41610</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="B5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -264,22 +288,22 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -305,7 +329,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
working on auto setup
</commit_message>
<xml_diff>
--- a/gantt-tj3/gantt-tj3.xlsx
+++ b/gantt-tj3/gantt-tj3.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Container_Task</t>
   </si>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t>Test 2 tj3 B</t>
+  </si>
+  <si>
+    <t>Phase3</t>
+  </si>
+  <si>
+    <t>doing a lot</t>
+  </si>
+  <si>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>toC</t>
   </si>
   <si>
     <t>resource_id</t>
@@ -167,14 +179,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
+      <selection activeCell="F6" activeCellId="0" pane="topLeft" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -263,6 +275,23 @@
       </c>
       <c r="F5" s="0" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
+      <c r="A6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -284,16 +313,16 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
+      <selection activeCell="A3" activeCellId="1" pane="topLeft" sqref="F6 A3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="2">
@@ -325,11 +354,11 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="F6 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
at a good stage
</commit_message>
<xml_diff>
--- a/gantt-tj3/gantt-tj3.xlsx
+++ b/gantt-tj3/gantt-tj3.xlsx
@@ -182,7 +182,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F6" activeCellId="0" pane="topLeft" sqref="F6"/>
+      <selection activeCell="F4" activeCellId="0" pane="topLeft" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -256,8 +256,8 @@
       <c r="E4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
+      <c r="F4" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="5">
@@ -313,7 +313,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="1" pane="topLeft" sqref="F6 A3"/>
+      <selection activeCell="A3" activeCellId="1" pane="topLeft" sqref="F4 A3"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -354,7 +354,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="F6 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="F4 A1"/>
     </sheetView>
   </sheetViews>
   <cols>

</xml_diff>

<commit_message>
change to gantt xls
</commit_message>
<xml_diff>
--- a/gantt-tj3/gantt-tj3.xlsx
+++ b/gantt-tj3/gantt-tj3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="141" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="191" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Action list" sheetId="1" state="visible" r:id="rId2"/>
@@ -227,11 +227,15 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F4" activeCellId="0" pane="topLeft" sqref="F4"/>
+      <selection activeCell="A2" activeCellId="0" pane="topLeft" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2117647058824"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.2117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -446,7 +450,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>33</v>
       </c>
@@ -485,11 +489,11 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A3" activeCellId="1" pane="topLeft" sqref="F4 A3"/>
+      <selection activeCell="A3" activeCellId="0" pane="topLeft" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -526,11 +530,11 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="F4 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.9843137254902"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>